<commit_message>
Added download template and validations to uploadStamping
</commit_message>
<xml_diff>
--- a/template/Stamping Record Template.xlsx
+++ b/template/Stamping Record Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\scm\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6018588B-8272-4BC9-B565-689D4B7117BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F379045-CAD4-401F-957B-8B418DDF03A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2022 (DUE 2023) A-M'!$A$2:$S$1399</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$S$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -764,7 +764,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9913" uniqueCount="2820">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9919" uniqueCount="2826">
   <si>
     <t>Customer (A-M)</t>
   </si>
@@ -9085,9 +9085,6 @@
     <t>Dealer</t>
   </si>
   <si>
-    <t>Dealer Branch</t>
-  </si>
-  <si>
     <t>Customer Type</t>
   </si>
   <si>
@@ -9251,6 +9248,27 @@
   </si>
   <si>
     <t>Total Charges</t>
+  </si>
+  <si>
+    <t>Address Line 1</t>
+  </si>
+  <si>
+    <t>Address Line 4</t>
+  </si>
+  <si>
+    <t>Address Line 3</t>
+  </si>
+  <si>
+    <t>Address Line 2</t>
+  </si>
+  <si>
+    <t>Tel</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Other Code</t>
   </si>
 </sst>
 </file>
@@ -9261,7 +9279,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;RM&quot;* #,##0.00_-;\-&quot;RM&quot;* #,##0.00_-;_-&quot;RM&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-409]dd\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -9374,6 +9392,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -9632,7 +9657,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -9926,6 +9951,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -10227,267 +10253,311 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BL1"/>
+  <dimension ref="A1:BR1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BC1" workbookViewId="0">
-      <selection activeCell="BL9" sqref="BL9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:BP1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="50" max="51" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="4" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="15" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="14.42578125" customWidth="1"/>
+    <col min="12" max="12" width="3.7109375" customWidth="1"/>
+    <col min="13" max="13" width="5.85546875" customWidth="1"/>
+    <col min="14" max="14" width="3.85546875" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" customWidth="1"/>
+    <col min="16" max="16" width="6.140625" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" customWidth="1"/>
+    <col min="18" max="18" width="6.7109375" customWidth="1"/>
+    <col min="19" max="19" width="8" customWidth="1"/>
+    <col min="20" max="20" width="8.42578125" customWidth="1"/>
+    <col min="21" max="21" width="9" customWidth="1"/>
+    <col min="22" max="22" width="9.28515625" customWidth="1"/>
+    <col min="23" max="24" width="10.7109375" customWidth="1"/>
+    <col min="25" max="25" width="16.7109375" customWidth="1"/>
+    <col min="26" max="26" width="14.140625" customWidth="1"/>
+    <col min="27" max="27" width="11" customWidth="1"/>
+    <col min="28" max="28" width="10" customWidth="1"/>
+    <col min="29" max="29" width="9.42578125" customWidth="1"/>
+    <col min="30" max="30" width="14.42578125" customWidth="1"/>
+    <col min="31" max="31" width="16.5703125" customWidth="1"/>
+    <col min="32" max="32" width="13.28515625" customWidth="1"/>
+    <col min="33" max="33" width="17.28515625" customWidth="1"/>
+    <col min="34" max="34" width="6" customWidth="1"/>
+    <col min="35" max="35" width="14" customWidth="1"/>
+    <col min="36" max="37" width="15.85546875" customWidth="1"/>
+    <col min="38" max="38" width="12.140625" customWidth="1"/>
+    <col min="39" max="39" width="15.7109375" customWidth="1"/>
+    <col min="40" max="40" width="11.7109375" customWidth="1"/>
+    <col min="41" max="41" width="7.7109375" customWidth="1"/>
+    <col min="43" max="43" width="10.42578125" customWidth="1"/>
+    <col min="44" max="44" width="20.7109375" customWidth="1"/>
+    <col min="45" max="45" width="19.42578125" customWidth="1"/>
+    <col min="46" max="46" width="18.140625" customWidth="1"/>
+    <col min="47" max="47" width="8.42578125" customWidth="1"/>
+    <col min="48" max="48" width="14" customWidth="1"/>
+    <col min="49" max="49" width="9.140625" customWidth="1"/>
+    <col min="50" max="50" width="13.140625" customWidth="1"/>
+    <col min="51" max="51" width="14.7109375" customWidth="1"/>
+    <col min="52" max="52" width="12" customWidth="1"/>
+    <col min="53" max="53" width="13.7109375" customWidth="1"/>
+    <col min="54" max="54" width="8.5703125" customWidth="1"/>
+    <col min="55" max="55" width="15.28515625" customWidth="1"/>
+    <col min="56" max="56" width="16.140625" customWidth="1"/>
+    <col min="57" max="58" width="9.5703125" customWidth="1"/>
+    <col min="59" max="59" width="13.140625" customWidth="1"/>
+    <col min="60" max="60" width="4" customWidth="1"/>
+    <col min="61" max="61" width="19.7109375" customWidth="1"/>
+    <col min="63" max="63" width="15" customWidth="1"/>
+    <col min="64" max="64" width="16.140625" customWidth="1"/>
+    <col min="65" max="65" width="13.7109375" customWidth="1"/>
+    <col min="66" max="66" width="23.7109375" customWidth="1"/>
+    <col min="67" max="67" width="12.42578125" customWidth="1"/>
+    <col min="68" max="68" width="12.85546875" customWidth="1"/>
+    <col min="69" max="69" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+    <row r="1" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A1" s="99" t="s">
         <v>2761</v>
       </c>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="99" t="s">
         <v>2762</v>
       </c>
-      <c r="C1" s="95" t="s">
+      <c r="C1" s="99" t="s">
         <v>2763</v>
       </c>
-      <c r="D1" s="95" t="s">
+      <c r="D1" s="99" t="s">
         <v>2764</v>
       </c>
-      <c r="E1" s="95" t="s">
+      <c r="E1" s="99" t="s">
         <v>2765</v>
       </c>
-      <c r="F1" s="95" t="s">
+      <c r="F1" s="99" t="s">
         <v>2766</v>
       </c>
-      <c r="G1" s="95" t="s">
+      <c r="G1" s="99" t="s">
+        <v>2825</v>
+      </c>
+      <c r="H1" s="99" t="s">
+        <v>2819</v>
+      </c>
+      <c r="I1" s="99" t="s">
+        <v>2822</v>
+      </c>
+      <c r="J1" s="99" t="s">
+        <v>2821</v>
+      </c>
+      <c r="K1" s="99" t="s">
+        <v>2820</v>
+      </c>
+      <c r="L1" s="99" t="s">
+        <v>2823</v>
+      </c>
+      <c r="M1" s="99" t="s">
+        <v>2824</v>
+      </c>
+      <c r="N1" s="99" t="s">
+        <v>2797</v>
+      </c>
+      <c r="O1" s="99" t="s">
+        <v>2798</v>
+      </c>
+      <c r="P1" s="99" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="99" t="s">
         <v>2767</v>
       </c>
-      <c r="H1" s="95" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="95" t="s">
+      <c r="R1" s="99" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" s="99" t="s">
         <v>2768</v>
       </c>
-      <c r="J1" s="95" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="95" t="s">
+      <c r="T1" s="99" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" s="99" t="s">
         <v>2769</v>
       </c>
-      <c r="L1" s="95" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="95" t="s">
+      <c r="V1" s="99" t="s">
         <v>2770</v>
       </c>
-      <c r="N1" s="95" t="s">
+      <c r="W1" s="99" t="s">
         <v>2771</v>
       </c>
-      <c r="O1" s="95" t="s">
+      <c r="X1" s="99" t="s">
         <v>2772</v>
       </c>
-      <c r="P1" s="95" t="s">
+      <c r="Y1" s="99" t="s">
         <v>2773</v>
       </c>
-      <c r="Q1" s="95" t="s">
+      <c r="Z1" s="99" t="s">
+        <v>2814</v>
+      </c>
+      <c r="AA1" s="99" t="s">
         <v>2774</v>
       </c>
-      <c r="R1" s="95" t="s">
+      <c r="AB1" s="99" t="s">
         <v>2775</v>
       </c>
-      <c r="S1" s="95" t="s">
+      <c r="AC1" s="99" t="s">
         <v>2776</v>
       </c>
-      <c r="T1" s="95" t="s">
+      <c r="AD1" s="99" t="s">
         <v>2777</v>
       </c>
-      <c r="U1" s="95" t="s">
+      <c r="AE1" s="99" t="s">
         <v>2778</v>
       </c>
-      <c r="V1" s="95" t="s">
+      <c r="AF1" s="99" t="s">
         <v>2779</v>
       </c>
-      <c r="W1" s="95" t="s">
+      <c r="AG1" s="99" t="s">
         <v>2780</v>
       </c>
-      <c r="X1" s="95" t="s">
+      <c r="AH1" s="99" t="s">
         <v>2781</v>
       </c>
-      <c r="Y1" s="95" t="s">
+      <c r="AI1" s="99" t="s">
         <v>2782</v>
       </c>
-      <c r="Z1" s="95" t="s">
+      <c r="AJ1" s="99" t="s">
         <v>2783</v>
       </c>
-      <c r="AA1" s="95" t="s">
+      <c r="AK1" s="99" t="s">
         <v>2784</v>
       </c>
-      <c r="AB1" s="95" t="s">
+      <c r="AL1" s="99" t="s">
         <v>2785</v>
       </c>
-      <c r="AC1" s="95" t="s">
+      <c r="AM1" s="99" t="s">
         <v>2786</v>
       </c>
-      <c r="AD1" s="95" t="s">
+      <c r="AN1" s="99" t="s">
         <v>2787</v>
       </c>
-      <c r="AE1" s="95" t="s">
+      <c r="AO1" s="99" t="s">
         <v>2788</v>
       </c>
-      <c r="AF1" s="95" t="s">
+      <c r="AP1" s="99" t="s">
         <v>2789</v>
       </c>
-      <c r="AG1" s="95" t="s">
+      <c r="AQ1" s="99" t="s">
         <v>2790</v>
       </c>
-      <c r="AH1" s="95" t="s">
+      <c r="AR1" s="99" t="s">
         <v>2791</v>
       </c>
-      <c r="AI1" s="95" t="s">
+      <c r="AS1" s="99" t="s">
         <v>2792</v>
       </c>
-      <c r="AJ1" s="95" t="s">
+      <c r="AT1" s="99" t="s">
         <v>2793</v>
       </c>
-      <c r="AK1" s="95" t="s">
+      <c r="AU1" s="99" t="s">
         <v>2794</v>
       </c>
-      <c r="AL1" s="95" t="s">
+      <c r="AV1" s="99" t="s">
         <v>2795</v>
       </c>
-      <c r="AM1" s="95" t="s">
+      <c r="AW1" s="99" t="s">
         <v>2796</v>
       </c>
-      <c r="AN1" s="95" t="s">
-        <v>2797</v>
-      </c>
-      <c r="AO1" s="95" t="s">
-        <v>2798</v>
-      </c>
-      <c r="AP1" s="95" t="s">
+      <c r="AX1" s="99" t="s">
         <v>2799</v>
       </c>
-      <c r="AQ1" s="95" t="s">
+      <c r="AY1" s="99" t="s">
         <v>2800</v>
       </c>
-      <c r="AR1" s="95" t="s">
+      <c r="AZ1" s="99" t="s">
         <v>2801</v>
       </c>
-      <c r="AS1" s="95" t="s">
+      <c r="BA1" s="99" t="s">
         <v>2802</v>
       </c>
-      <c r="AT1" s="95" t="s">
+      <c r="BB1" s="99" t="s">
         <v>2803</v>
       </c>
-      <c r="AU1" s="95" t="s">
+      <c r="BC1" s="99" t="s">
         <v>2804</v>
       </c>
-      <c r="AV1" s="95" t="s">
+      <c r="BD1" s="99" t="s">
         <v>2805</v>
       </c>
-      <c r="AW1" s="95" t="s">
+      <c r="BE1" s="99" t="s">
         <v>2806</v>
       </c>
-      <c r="AX1" s="95" t="s">
+      <c r="BF1" s="99" t="s">
         <v>2807</v>
       </c>
-      <c r="AY1" s="95" t="s">
+      <c r="BG1" s="99" t="s">
         <v>2808</v>
       </c>
-      <c r="AZ1" s="95" t="s">
+      <c r="BH1" s="99" t="s">
         <v>2809</v>
       </c>
-      <c r="BA1" s="95" t="s">
+      <c r="BI1" s="99" t="s">
         <v>2810</v>
       </c>
-      <c r="BB1" s="95" t="s">
+      <c r="BJ1" s="99" t="s">
         <v>2811</v>
       </c>
-      <c r="BC1" s="95" t="s">
+      <c r="BK1" s="99" t="s">
         <v>2812</v>
       </c>
-      <c r="BD1" s="95" t="s">
+      <c r="BL1" s="99" t="s">
         <v>2813</v>
       </c>
-      <c r="BE1" s="95" t="s">
-        <v>2814</v>
-      </c>
-      <c r="BF1" s="95" t="s">
+      <c r="BM1" s="99" t="s">
         <v>2815</v>
       </c>
-      <c r="BG1" s="95" t="s">
+      <c r="BN1" s="99" t="s">
         <v>2816</v>
       </c>
-      <c r="BH1" s="95" t="s">
+      <c r="BO1" s="99" t="s">
         <v>2817</v>
       </c>
-      <c r="BI1" s="95" t="s">
+      <c r="BP1" s="99" t="s">
         <v>2818</v>
       </c>
-      <c r="BJ1" s="95" t="s">
-        <v>2819</v>
-      </c>
-      <c r="BK1" s="95"/>
-      <c r="BL1" s="95"/>
+      <c r="BQ1" s="95"/>
+      <c r="BR1" s="95"/>
     </row>
   </sheetData>
+  <dataValidations count="7">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{BA917934-471F-497A-9293-322A7599E0FF}">
+      <formula1>"DIRECT, RESELLER"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576 E2:E1048576" xr:uid="{F52F65B7-19F8-48BB-80D3-455F4312AB62}">
+      <formula1>"NEW, EXISTING"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y1:Y1048576" xr:uid="{8A0F5E08-0C0A-4D6F-8E6B-04DFD3895B30}">
+      <formula1>"RENT, OWN"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z1:Z1048576" xr:uid="{5E7CAF4D-9AB1-41F1-83CC-ED777DA84C9D}">
+      <formula1>"NEW, RENEWAL"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH1:AH1048576" xr:uid="{3AD16212-0522-4B3C-BA7D-6CA0D0820960}">
+      <formula1>"TRADE,NON-TRADE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN1:AN1048576" xr:uid="{F924DC67-0A6B-4720-8544-8C16E8BAAB0D}">
+      <formula1>"YES,NO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR1:AR1048576" xr:uid="{3F755542-5F99-46C3-9917-919BE0B46990}">
+      <formula1>"Cash,Check,Online"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>